<commit_message>
add keywords and update pickle trial
</commit_message>
<xml_diff>
--- a/Corpus/MLR_Corpus.xlsx
+++ b/Corpus/MLR_Corpus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CleverBrain\Nuplazid\Masori-Chatbot-UAT\Corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCA81A2-EBB6-4119-9054-A831F44B56DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2D65A4-238A-4FBD-BBB5-5ADD01DE0599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1455,10 +1455,10 @@
     <t>Real-World Evidence</t>
   </si>
   <si>
-    <t>real-world-evidence</t>
-  </si>
-  <si>
     <t>Real World Data, Mortality Data, Mosholder Study, Layton Study</t>
+  </si>
+  <si>
+    <t>https://www.nuplazidhcp.com/real-world-evidence</t>
   </si>
 </sst>
 </file>
@@ -1604,24 +1604,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1629,20 +1629,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2082,13 +2082,13 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>242</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -2106,14 +2106,14 @@
       <c r="L2" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="27" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2129,12 +2129,12 @@
       <c r="L3" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="M3" s="22"/>
+      <c r="M3" s="25"/>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="1" t="s">
         <v>292</v>
       </c>
@@ -2150,16 +2150,16 @@
       <c r="L4" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M4" s="22"/>
+      <c r="M4" s="25"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="21" t="s">
         <v>205</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2177,14 +2177,14 @@
       <c r="L5" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="24" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="1" t="s">
         <v>274</v>
       </c>
@@ -2200,16 +2200,16 @@
       <c r="L6" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M6" s="22"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="21" t="s">
         <v>259</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -2227,14 +2227,14 @@
       <c r="L7" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="24" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="1" t="s">
         <v>258</v>
       </c>
@@ -2250,12 +2250,12 @@
       <c r="L8" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="M8" s="22"/>
+      <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="1" t="s">
         <v>260</v>
       </c>
@@ -2268,12 +2268,12 @@
       <c r="L9" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="M9" s="22"/>
+      <c r="M9" s="25"/>
     </row>
     <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="1" t="s">
         <v>331</v>
       </c>
@@ -2354,13 +2354,13 @@
       <c r="M14" s="13"/>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="21" t="s">
         <v>252</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2378,14 +2378,14 @@
       <c r="L15" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M15" s="23" t="s">
+      <c r="M15" s="24" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="1" t="s">
         <v>295</v>
       </c>
@@ -2401,12 +2401,12 @@
       <c r="L16" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M16" s="22"/>
+      <c r="M16" s="25"/>
     </row>
     <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="1" t="s">
         <v>296</v>
       </c>
@@ -2422,12 +2422,12 @@
       <c r="L17" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M17" s="22"/>
+      <c r="M17" s="25"/>
     </row>
     <row r="18" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="1" t="s">
         <v>301</v>
       </c>
@@ -2439,16 +2439,16 @@
       </c>
       <c r="G18" s="1"/>
       <c r="L18" s="15"/>
-      <c r="M18" s="22"/>
+      <c r="M18" s="25"/>
     </row>
     <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="21" t="s">
         <v>208</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -2466,14 +2466,14 @@
       <c r="L19" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M19" s="23" t="s">
+      <c r="M19" s="24" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="1" t="s">
         <v>298</v>
       </c>
@@ -2489,12 +2489,12 @@
       <c r="L20" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M20" s="22"/>
+      <c r="M20" s="25"/>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="26"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="1" t="s">
         <v>175</v>
       </c>
@@ -2510,12 +2510,12 @@
       <c r="L21" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M21" s="22"/>
+      <c r="M21" s="25"/>
     </row>
     <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="26"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="1" t="s">
         <v>176</v>
       </c>
@@ -2531,16 +2531,16 @@
       <c r="L22" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="M22" s="22"/>
+      <c r="M22" s="25"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="21" t="s">
         <v>209</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -2555,14 +2555,14 @@
       <c r="L23" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="M23" s="23" t="s">
+      <c r="M23" s="24" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="1" t="s">
         <v>18</v>
       </c>
@@ -2578,12 +2578,12 @@
       <c r="L24" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M24" s="22"/>
+      <c r="M24" s="25"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="1" t="s">
         <v>254</v>
       </c>
@@ -2598,12 +2598,12 @@
       <c r="L25" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="M25" s="22"/>
+      <c r="M25" s="25"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="1" t="s">
         <v>66</v>
       </c>
@@ -2619,16 +2619,16 @@
       <c r="L26" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="M26" s="22"/>
+      <c r="M26" s="25"/>
     </row>
     <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="26" t="s">
         <v>211</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -2645,14 +2645,14 @@
       <c r="L27" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="M27" s="23" t="s">
+      <c r="M27" s="24" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="27"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="1" t="s">
         <v>179</v>
       </c>
@@ -2668,19 +2668,19 @@
       <c r="L28" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M28" s="22"/>
+      <c r="M28" s="25"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="27"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="26"/>
       <c r="L29" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="M29" s="22"/>
+      <c r="M29" s="25"/>
     </row>
     <row r="30" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="23" t="s">
         <v>180</v>
       </c>
       <c r="C30" s="1"/>
@@ -2696,16 +2696,16 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="15"/>
-      <c r="M30" s="23" t="s">
+      <c r="M30" s="24" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="25" t="s">
+      <c r="A31" s="23"/>
+      <c r="B31" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="21" t="s">
         <v>213</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -2723,12 +2723,12 @@
       <c r="L31" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M31" s="22"/>
+      <c r="M31" s="25"/>
     </row>
     <row r="32" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="25"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="1" t="s">
         <v>306</v>
       </c>
@@ -2743,12 +2743,12 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="15"/>
-      <c r="M32" s="22"/>
+      <c r="M32" s="25"/>
     </row>
     <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="1" t="s">
         <v>299</v>
       </c>
@@ -2761,12 +2761,12 @@
       <c r="L33" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="M33" s="22"/>
+      <c r="M33" s="25"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="25"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="1" t="s">
         <v>172</v>
       </c>
@@ -2782,12 +2782,12 @@
       <c r="L34" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="M34" s="22"/>
+      <c r="M34" s="25"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="1" t="s">
         <v>202</v>
       </c>
@@ -2803,12 +2803,12 @@
       <c r="L35" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="M35" s="22"/>
+      <c r="M35" s="25"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="25"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="1" t="s">
         <v>180</v>
       </c>
@@ -2821,16 +2821,16 @@
       <c r="L36" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="M36" s="22"/>
+      <c r="M36" s="25"/>
     </row>
     <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="21" t="s">
         <v>216</v>
       </c>
       <c r="D37" s="1" t="s">
@@ -2848,14 +2848,14 @@
       <c r="L37" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M37" s="23" t="s">
+      <c r="M37" s="24" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="23"/>
       <c r="D38" s="1" t="s">
         <v>182</v>
       </c>
@@ -2871,12 +2871,12 @@
       <c r="L38" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M38" s="22"/>
+      <c r="M38" s="25"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="26"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="23"/>
       <c r="D39" s="1" t="s">
         <v>183</v>
       </c>
@@ -2884,24 +2884,24 @@
       <c r="L39" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M39" s="22"/>
+      <c r="M39" s="25"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="26"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="23"/>
       <c r="D40" s="1" t="s">
         <v>184</v>
       </c>
       <c r="L40" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M40" s="22"/>
+      <c r="M40" s="25"/>
     </row>
     <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="26"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="23"/>
       <c r="D41" s="1" t="s">
         <v>185</v>
       </c>
@@ -2917,12 +2917,12 @@
       <c r="L41" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M41" s="22"/>
+      <c r="M41" s="25"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="26"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="23"/>
       <c r="D42" s="1" t="s">
         <v>277</v>
       </c>
@@ -2938,12 +2938,12 @@
       <c r="L42" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="M42" s="22"/>
+      <c r="M42" s="25"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="26"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="23"/>
       <c r="D43" s="1" t="s">
         <v>187</v>
       </c>
@@ -2959,7 +2959,7 @@
       <c r="L43" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="M43" s="22"/>
+      <c r="M43" s="25"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -3010,6 +3010,33 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="M19:M22"/>
+    <mergeCell ref="M23:M26"/>
+    <mergeCell ref="M7:M9"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="C37:C43"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="M30:M36"/>
+    <mergeCell ref="M37:M43"/>
+    <mergeCell ref="M27:M29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B27:B29"/>
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A30:A36"/>
@@ -3019,33 +3046,6 @@
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B37:B43"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="C37:C43"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="M30:M36"/>
-    <mergeCell ref="M37:M43"/>
-    <mergeCell ref="M27:M29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="M19:M22"/>
-    <mergeCell ref="M23:M26"/>
-    <mergeCell ref="M7:M9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" display="https://www.nuplazid.com/about-pd-related-hallucinations-and-delusions" xr:uid="{8B199CA5-51D2-4A5F-A317-094F7584A959}"/>
@@ -3456,7 +3456,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="26" t="s">
         <v>58</v>
       </c>
       <c r="D37" t="s">
@@ -3464,43 +3464,43 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
+      <c r="A38" s="26"/>
       <c r="D38" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
+      <c r="A39" s="26"/>
       <c r="D39" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
+      <c r="A40" s="26"/>
       <c r="D40" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
+      <c r="A41" s="26"/>
       <c r="D41" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
+      <c r="A42" s="26"/>
       <c r="D42" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
+      <c r="A43" s="26"/>
       <c r="D43" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="26" t="s">
         <v>66</v>
       </c>
       <c r="C44" t="s">
@@ -3511,7 +3511,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
+      <c r="A45" s="26"/>
       <c r="C45" t="s">
         <v>67</v>
       </c>
@@ -3520,7 +3520,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
+      <c r="A46" s="26"/>
       <c r="C46" t="s">
         <v>44</v>
       </c>
@@ -3529,43 +3529,43 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
+      <c r="A47" s="26"/>
       <c r="D47" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
+      <c r="A48" s="26"/>
       <c r="D48" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
+      <c r="A49" s="26"/>
       <c r="D49" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
+      <c r="A50" s="26"/>
       <c r="D50" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
+      <c r="A51" s="26"/>
       <c r="D51" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
+      <c r="A52" s="26"/>
       <c r="D52" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="158.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
+      <c r="A53" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C53" t="s">
@@ -3576,7 +3576,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
+      <c r="A54" s="26"/>
       <c r="C54" t="s">
         <v>87</v>
       </c>
@@ -3585,7 +3585,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="s">
+      <c r="A55" s="26" t="s">
         <v>80</v>
       </c>
       <c r="C55" t="s">
@@ -3596,7 +3596,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="27"/>
+      <c r="A56" s="26"/>
       <c r="C56" t="s">
         <v>82</v>
       </c>
@@ -3605,7 +3605,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="27"/>
+      <c r="A57" s="26"/>
       <c r="C57" t="s">
         <v>83</v>
       </c>
@@ -3614,7 +3614,7 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="27"/>
+      <c r="A58" s="26"/>
       <c r="C58" t="s">
         <v>84</v>
       </c>
@@ -3623,7 +3623,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
+      <c r="A59" s="26"/>
       <c r="C59" t="s">
         <v>85</v>
       </c>
@@ -3632,73 +3632,73 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
+      <c r="A60" s="26"/>
       <c r="D60" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="27"/>
+      <c r="A61" s="26"/>
       <c r="D61" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="27"/>
+      <c r="A62" s="26"/>
       <c r="D62" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="27"/>
+      <c r="A63" s="26"/>
       <c r="D63" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="27"/>
+      <c r="A64" s="26"/>
       <c r="D64" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="27"/>
+      <c r="A65" s="26"/>
       <c r="D65" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="27"/>
+      <c r="A66" s="26"/>
       <c r="D66" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
+      <c r="A67" s="26"/>
       <c r="D67" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="27"/>
+      <c r="A68" s="26"/>
       <c r="D68" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="27"/>
+      <c r="A69" s="26"/>
       <c r="D69" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="27"/>
+      <c r="A70" s="26"/>
       <c r="D70" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="27" t="s">
+      <c r="A71" s="26" t="s">
         <v>104</v>
       </c>
       <c r="C71" t="s">
@@ -3709,7 +3709,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
+      <c r="A72" s="26"/>
       <c r="C72" t="s">
         <v>106</v>
       </c>
@@ -3718,7 +3718,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="27"/>
+      <c r="A73" s="26"/>
       <c r="C73" t="s">
         <v>107</v>
       </c>
@@ -3727,7 +3727,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="27"/>
+      <c r="A74" s="26"/>
       <c r="C74" t="s">
         <v>108</v>
       </c>
@@ -3736,43 +3736,43 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="27"/>
+      <c r="A75" s="26"/>
       <c r="D75" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
+      <c r="A76" s="26"/>
       <c r="D76" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="27"/>
+      <c r="A77" s="26"/>
       <c r="D77" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
+      <c r="A78" s="26"/>
       <c r="D78" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="27"/>
+      <c r="A79" s="26"/>
       <c r="D79" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="27"/>
+      <c r="A80" s="26"/>
       <c r="D80" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="27" t="s">
+      <c r="A81" s="26" t="s">
         <v>117</v>
       </c>
       <c r="C81" t="s">
@@ -3783,7 +3783,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="27"/>
+      <c r="A82" s="26"/>
       <c r="C82" t="s">
         <v>119</v>
       </c>
@@ -3792,7 +3792,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="27"/>
+      <c r="A83" s="26"/>
       <c r="C83" t="s">
         <v>120</v>
       </c>
@@ -3801,25 +3801,25 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="27"/>
+      <c r="A84" s="26"/>
       <c r="D84" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="27"/>
+      <c r="A85" s="26"/>
       <c r="D85" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="27"/>
+      <c r="A86" s="26"/>
       <c r="D86" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="27" t="s">
+      <c r="A87" s="26" t="s">
         <v>125</v>
       </c>
       <c r="C87" t="s">
@@ -3830,7 +3830,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A88" s="27"/>
+      <c r="A88" s="26"/>
       <c r="C88" t="s">
         <v>127</v>
       </c>
@@ -3839,7 +3839,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="27"/>
+      <c r="A89" s="26"/>
       <c r="C89" t="s">
         <v>128</v>
       </c>
@@ -3848,13 +3848,13 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="27"/>
+      <c r="A90" s="26"/>
       <c r="C90" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A91" s="27" t="s">
+      <c r="A91" s="26" t="s">
         <v>132</v>
       </c>
       <c r="C91" t="s">
@@ -3865,7 +3865,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A92" s="27"/>
+      <c r="A92" s="26"/>
       <c r="C92" t="s">
         <v>134</v>
       </c>
@@ -3874,37 +3874,37 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="27"/>
+      <c r="A93" s="26"/>
       <c r="C93" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="27"/>
+      <c r="A94" s="26"/>
       <c r="C94" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="27"/>
+      <c r="A95" s="26"/>
       <c r="C95" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="27"/>
+      <c r="A96" s="26"/>
       <c r="C96" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="27"/>
+      <c r="A97" s="26"/>
       <c r="C97" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="27" t="s">
+      <c r="A98" s="26" t="s">
         <v>141</v>
       </c>
       <c r="D98" t="s">
@@ -3912,25 +3912,25 @@
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="27"/>
+      <c r="A99" s="26"/>
       <c r="D99" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="27"/>
+      <c r="A100" s="26"/>
       <c r="D100" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="27"/>
+      <c r="A101" s="26"/>
       <c r="D101" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="27" t="s">
+      <c r="A102" s="26" t="s">
         <v>146</v>
       </c>
       <c r="C102" t="s">
@@ -3941,7 +3941,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="27"/>
+      <c r="A103" s="26"/>
       <c r="C103" t="s">
         <v>138</v>
       </c>
@@ -3950,7 +3950,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="27"/>
+      <c r="A104" s="26"/>
       <c r="C104" t="s">
         <v>135</v>
       </c>
@@ -3959,7 +3959,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="27"/>
+      <c r="A105" s="26"/>
       <c r="C105" t="s">
         <v>147</v>
       </c>
@@ -3968,7 +3968,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="27"/>
+      <c r="A106" s="26"/>
       <c r="C106" t="s">
         <v>148</v>
       </c>
@@ -3977,13 +3977,13 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="27"/>
+      <c r="A107" s="26"/>
       <c r="C107" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="27" t="s">
+      <c r="A108" s="26" t="s">
         <v>151</v>
       </c>
       <c r="C108" t="s">
@@ -3994,7 +3994,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="27"/>
+      <c r="A109" s="26"/>
       <c r="C109" t="s">
         <v>153</v>
       </c>
@@ -4003,31 +4003,31 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="27"/>
+      <c r="A110" s="26"/>
       <c r="D110" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="27"/>
+      <c r="A111" s="26"/>
       <c r="D111" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="27"/>
+      <c r="A112" s="26"/>
       <c r="D112" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="27"/>
+      <c r="A113" s="26"/>
       <c r="D113" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="27" t="s">
+      <c r="A114" s="26" t="s">
         <v>163</v>
       </c>
       <c r="C114" t="s">
@@ -4038,7 +4038,7 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="27"/>
+      <c r="A115" s="26"/>
       <c r="C115" t="s">
         <v>119</v>
       </c>
@@ -4047,7 +4047,7 @@
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="27"/>
+      <c r="A116" s="26"/>
       <c r="C116" t="s">
         <v>120</v>
       </c>
@@ -4056,55 +4056,55 @@
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="27"/>
+      <c r="A117" s="26"/>
       <c r="D117" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="27"/>
+      <c r="A118" s="26"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="27"/>
+      <c r="A119" s="26"/>
       <c r="D119" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="27"/>
+      <c r="A120" s="26"/>
       <c r="D120" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="27"/>
+      <c r="A121" s="26"/>
       <c r="D121" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="27"/>
+      <c r="A122" s="26"/>
       <c r="D122" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="27"/>
+      <c r="A123" s="26"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="27"/>
+      <c r="A124" s="26"/>
       <c r="D124" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A125" s="27"/>
+      <c r="A125" s="26"/>
       <c r="D125" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="27"/>
+      <c r="A126" s="26"/>
       <c r="D126" t="s">
         <v>170</v>
       </c>
@@ -4142,9 +4142,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4204,7 +4204,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="28" t="s">
@@ -4233,7 +4233,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
       <c r="D3" s="1" t="s">
@@ -4257,19 +4257,19 @@
       <c r="A4" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -4278,17 +4278,17 @@
       <c r="L4" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="24" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -4297,15 +4297,15 @@
       <c r="L5" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M5" s="22"/>
+      <c r="M5" s="25"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -4314,15 +4314,15 @@
       <c r="L6" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M6" s="22"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -4331,15 +4331,15 @@
       <c r="L7" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M7" s="22"/>
+      <c r="M7" s="25"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -4348,12 +4348,12 @@
       <c r="L8" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="M8" s="22"/>
+      <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
       <c r="D9" s="1" t="s">
         <v>304</v>
       </c>
@@ -4377,65 +4377,65 @@
       <c r="A10" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="30" t="s">
         <v>275</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="32" t="s">
+      <c r="F10" s="21"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="24" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="22"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="22"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="27"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="1" t="s">
         <v>334</v>
       </c>
@@ -4451,12 +4451,12 @@
       <c r="L13" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M13" s="22"/>
+      <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="29"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="27"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
@@ -4472,12 +4472,12 @@
       <c r="L14" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M14" s="22"/>
+      <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="27"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -4487,12 +4487,12 @@
       <c r="J15" s="15"/>
       <c r="K15" s="1"/>
       <c r="L15" s="15"/>
-      <c r="M15" s="22"/>
+      <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="27"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -4502,16 +4502,16 @@
       <c r="J16" s="15"/>
       <c r="K16" s="1"/>
       <c r="L16" s="15"/>
-      <c r="M16" s="22"/>
+      <c r="M16" s="25"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="26" t="s">
         <v>220</v>
       </c>
       <c r="D17" s="1"/>
@@ -4523,14 +4523,14 @@
       <c r="J17" s="15"/>
       <c r="K17" s="1"/>
       <c r="L17" s="15"/>
-      <c r="M17" s="23" t="s">
+      <c r="M17" s="24" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -4540,24 +4540,24 @@
       <c r="J18" s="15"/>
       <c r="K18" s="1"/>
       <c r="L18" s="15"/>
-      <c r="M18" s="23"/>
+      <c r="M18" s="24"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="15"/>
       <c r="L19" s="15"/>
-      <c r="M19" s="23"/>
+      <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -4567,12 +4567,12 @@
       <c r="J20" s="15"/>
       <c r="K20" s="1"/>
       <c r="L20" s="15"/>
-      <c r="M20" s="23"/>
+      <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="29"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
       <c r="D21" s="1" t="s">
         <v>45</v>
       </c>
@@ -4586,12 +4586,12 @@
       <c r="L21" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M21" s="23"/>
+      <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="1" t="s">
         <v>290</v>
       </c>
@@ -4607,12 +4607,12 @@
       <c r="L22" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M22" s="23"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -4623,12 +4623,12 @@
       <c r="L23" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M23" s="23"/>
+      <c r="M23" s="24"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="1" t="s">
         <v>192</v>
       </c>
@@ -4644,12 +4644,12 @@
       <c r="L24" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M24" s="23"/>
+      <c r="M24" s="24"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -4661,16 +4661,16 @@
       <c r="L25" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M25" s="23"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="26" t="s">
         <v>246</v>
       </c>
       <c r="F26" s="1"/>
@@ -4680,14 +4680,14 @@
       <c r="J26" s="15"/>
       <c r="K26" s="1"/>
       <c r="L26" s="15"/>
-      <c r="M26" s="23" t="s">
+      <c r="M26" s="24" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="1" t="s">
         <v>58</v>
       </c>
@@ -4703,12 +4703,12 @@
       <c r="L27" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M27" s="22"/>
+      <c r="M27" s="25"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -4719,12 +4719,12 @@
       <c r="L28" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="M28" s="22"/>
+      <c r="M28" s="25"/>
     </row>
     <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
       <c r="D29" s="1" t="s">
         <v>193</v>
       </c>
@@ -4740,16 +4740,16 @@
       <c r="L29" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="M29" s="22"/>
+      <c r="M29" s="25"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>222</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -4762,14 +4762,14 @@
       <c r="L30" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="M30" s="23" t="s">
+      <c r="M30" s="24" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="1" t="s">
         <v>67</v>
       </c>
@@ -4785,12 +4785,12 @@
       <c r="L31" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="M31" s="22"/>
+      <c r="M31" s="25"/>
     </row>
     <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="1" t="s">
         <v>44</v>
       </c>
@@ -4806,12 +4806,12 @@
       <c r="L32" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="M32" s="22"/>
+      <c r="M32" s="25"/>
     </row>
     <row r="33" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="1" t="s">
         <v>332</v>
       </c>
@@ -4825,12 +4825,12 @@
       <c r="L33" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="M33" s="22"/>
+      <c r="M33" s="25"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
       <c r="D34" s="1" t="s">
         <v>335</v>
       </c>
@@ -4844,12 +4844,12 @@
       <c r="L34" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="M34" s="22"/>
+      <c r="M34" s="25"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -4859,12 +4859,12 @@
       <c r="J35" s="15"/>
       <c r="K35" s="1"/>
       <c r="L35" s="15"/>
-      <c r="M35" s="22"/>
+      <c r="M35" s="25"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -4874,12 +4874,12 @@
       <c r="J36" s="15"/>
       <c r="K36" s="1"/>
       <c r="L36" s="15"/>
-      <c r="M36" s="22"/>
+      <c r="M36" s="25"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
       <c r="D37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -4888,16 +4888,16 @@
       <c r="J37" s="15"/>
       <c r="K37" s="1"/>
       <c r="L37" s="15"/>
-      <c r="M37" s="22"/>
+      <c r="M37" s="25"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B38" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="26" t="s">
         <v>223</v>
       </c>
       <c r="D38" s="1" t="s">
@@ -4915,14 +4915,14 @@
       <c r="L38" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="M38" s="23" t="s">
+      <c r="M38" s="24" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -4932,16 +4932,16 @@
       <c r="J39" s="15"/>
       <c r="K39" s="1"/>
       <c r="L39" s="15"/>
-      <c r="M39" s="22"/>
+      <c r="M39" s="25"/>
     </row>
     <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="26" t="s">
         <v>225</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -4956,14 +4956,14 @@
       <c r="L40" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="M40" s="23" t="s">
+      <c r="M40" s="24" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
       <c r="D41" s="1" t="s">
         <v>82</v>
       </c>
@@ -4974,12 +4974,12 @@
       <c r="L41" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="M41" s="22"/>
+      <c r="M41" s="25"/>
     </row>
     <row r="42" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
       <c r="D42" s="1" t="s">
         <v>83</v>
       </c>
@@ -4995,12 +4995,12 @@
       <c r="L42" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="M42" s="22"/>
+      <c r="M42" s="25"/>
     </row>
     <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
       <c r="D43" s="1" t="s">
         <v>85</v>
       </c>
@@ -5015,12 +5015,12 @@
       <c r="L43" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="M43" s="22"/>
+      <c r="M43" s="25"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
       <c r="D44" s="1" t="s">
         <v>276</v>
       </c>
@@ -5034,12 +5034,12 @@
       <c r="L44" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="M44" s="22"/>
+      <c r="M44" s="25"/>
     </row>
     <row r="45" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
       <c r="D45" s="1" t="s">
         <v>306</v>
       </c>
@@ -5055,124 +5055,124 @@
       <c r="J45" s="7"/>
       <c r="K45" s="1"/>
       <c r="L45" s="15"/>
-      <c r="M45" s="22"/>
+      <c r="M45" s="25"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="7"/>
       <c r="L46" s="15"/>
-      <c r="M46" s="22"/>
+      <c r="M46" s="25"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="7"/>
       <c r="L47" s="15"/>
-      <c r="M47" s="22"/>
+      <c r="M47" s="25"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="7"/>
       <c r="L48" s="15"/>
-      <c r="M48" s="22"/>
+      <c r="M48" s="25"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="7"/>
       <c r="L49" s="15"/>
-      <c r="M49" s="22"/>
+      <c r="M49" s="25"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="7"/>
       <c r="L50" s="15"/>
-      <c r="M50" s="22"/>
+      <c r="M50" s="25"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="7"/>
       <c r="L51" s="15"/>
-      <c r="M51" s="22"/>
+      <c r="M51" s="25"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="7"/>
       <c r="L52" s="15"/>
-      <c r="M52" s="22"/>
+      <c r="M52" s="25"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="7"/>
       <c r="L53" s="15"/>
-      <c r="M53" s="22"/>
+      <c r="M53" s="25"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="7"/>
       <c r="L54" s="15"/>
-      <c r="M54" s="22"/>
+      <c r="M54" s="25"/>
     </row>
     <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="s">
+      <c r="A55" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="B55" s="27" t="s">
+      <c r="B55" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="C55" s="27" t="s">
+      <c r="C55" s="26" t="s">
         <v>227</v>
       </c>
       <c r="D55" s="1" t="s">
@@ -5185,14 +5185,14 @@
       <c r="L55" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M55" s="32" t="s">
+      <c r="M55" s="31" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="27"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
       <c r="D56" s="1" t="s">
         <v>106</v>
       </c>
@@ -5203,12 +5203,12 @@
       <c r="L56" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M56" s="22"/>
+      <c r="M56" s="25"/>
     </row>
     <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="27"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
       <c r="D57" s="1" t="s">
         <v>107</v>
       </c>
@@ -5221,12 +5221,12 @@
       <c r="L57" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M57" s="22"/>
+      <c r="M57" s="25"/>
     </row>
     <row r="58" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="27"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
       <c r="D58" s="1" t="s">
         <v>108</v>
       </c>
@@ -5239,87 +5239,87 @@
       <c r="L58" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M58" s="22"/>
+      <c r="M58" s="25"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="7"/>
       <c r="L59" s="15"/>
-      <c r="M59" s="22"/>
+      <c r="M59" s="25"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="7"/>
       <c r="L60" s="15"/>
-      <c r="M60" s="22"/>
+      <c r="M60" s="25"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="27"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="7"/>
       <c r="L61" s="15"/>
-      <c r="M61" s="22"/>
+      <c r="M61" s="25"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="27"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="7"/>
       <c r="L62" s="15"/>
-      <c r="M62" s="22"/>
+      <c r="M62" s="25"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="27"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="27"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="7"/>
       <c r="L63" s="15"/>
-      <c r="M63" s="22"/>
+      <c r="M63" s="25"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="27"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="26"/>
+      <c r="C64" s="26"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="J64" s="7"/>
       <c r="L64" s="15"/>
-      <c r="M64" s="22"/>
+      <c r="M64" s="25"/>
     </row>
     <row r="65" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="27" t="s">
+      <c r="A65" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B65" s="27" t="s">
+      <c r="B65" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="C65" s="27" t="s">
+      <c r="C65" s="26" t="s">
         <v>250</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -5334,54 +5334,54 @@
       <c r="L65" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M65" s="32" t="s">
+      <c r="M65" s="31" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="27"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="7"/>
       <c r="L66" s="15"/>
-      <c r="M66" s="22"/>
+      <c r="M66" s="25"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="26"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="I67" s="1"/>
       <c r="J67" s="7"/>
       <c r="L67" s="15"/>
-      <c r="M67" s="22"/>
+      <c r="M67" s="25"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A68" s="27"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
+      <c r="A68" s="26"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="26"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="7"/>
       <c r="L68" s="15"/>
-      <c r="M68" s="22"/>
+      <c r="M68" s="25"/>
     </row>
     <row r="69" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="27" t="s">
+      <c r="A69" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B69" s="27" t="s">
+      <c r="B69" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="C69" s="27" t="s">
+      <c r="C69" s="26" t="s">
         <v>228</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -5396,14 +5396,14 @@
       <c r="L69" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M69" s="23" t="s">
+      <c r="M69" s="24" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="27"/>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
       <c r="D70" s="1" t="s">
         <v>127</v>
       </c>
@@ -5417,12 +5417,12 @@
       <c r="L70" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M70" s="22"/>
+      <c r="M70" s="25"/>
     </row>
     <row r="71" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="27"/>
-      <c r="B71" s="22"/>
-      <c r="C71" s="22"/>
+      <c r="A71" s="26"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
       <c r="D71" s="1" t="s">
         <v>128</v>
       </c>
@@ -5434,12 +5434,12 @@
       <c r="L71" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M71" s="22"/>
+      <c r="M71" s="25"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A72" s="27"/>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22"/>
+      <c r="A72" s="26"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
       <c r="D72" s="1" t="s">
         <v>277</v>
       </c>
@@ -5450,12 +5450,12 @@
       <c r="L72" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="M72" s="22"/>
+      <c r="M72" s="25"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A73" s="27"/>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22"/>
+      <c r="A73" s="26"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
       <c r="D73" s="1" t="s">
         <v>307</v>
       </c>
@@ -5466,47 +5466,47 @@
       <c r="L73" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="M73" s="22"/>
+      <c r="M73" s="25"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" s="27"/>
-      <c r="B74" s="22"/>
-      <c r="C74" s="22"/>
+      <c r="A74" s="26"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="7"/>
       <c r="L74" s="15"/>
-      <c r="M74" s="22"/>
+      <c r="M74" s="25"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A75" s="27"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="22"/>
+      <c r="A75" s="26"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="7"/>
       <c r="L75" s="15"/>
-      <c r="M75" s="22"/>
+      <c r="M75" s="25"/>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
-      <c r="B76" s="22"/>
-      <c r="C76" s="22"/>
+      <c r="A76" s="26"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
       <c r="F76" s="1"/>
-      <c r="M76" s="22"/>
+      <c r="M76" s="25"/>
     </row>
     <row r="77" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="27" t="s">
+      <c r="A77" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B77" s="27" t="s">
+      <c r="B77" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="C77" s="27" t="s">
+      <c r="C77" s="26" t="s">
         <v>230</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -5521,14 +5521,14 @@
       <c r="L77" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M77" s="32" t="s">
+      <c r="M77" s="31" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="27"/>
+      <c r="A78" s="26"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
       <c r="D78" s="1" t="s">
         <v>288</v>
       </c>
@@ -5539,16 +5539,16 @@
       <c r="L78" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M78" s="22"/>
+      <c r="M78" s="25"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="27" t="s">
+      <c r="A79" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="B79" s="27" t="s">
+      <c r="B79" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="C79" s="27" t="s">
+      <c r="C79" s="26" t="s">
         <v>232</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -5564,14 +5564,14 @@
       <c r="L79" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M79" s="32" t="s">
+      <c r="M79" s="31" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="27"/>
-      <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
+      <c r="A80" s="26"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="26"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -5579,40 +5579,40 @@
       <c r="I80" s="1"/>
       <c r="J80" s="15"/>
       <c r="L80" s="15"/>
-      <c r="M80" s="22"/>
+      <c r="M80" s="25"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" s="27"/>
-      <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
+      <c r="A81" s="26"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="15"/>
       <c r="L81" s="15"/>
-      <c r="M81" s="22"/>
+      <c r="M81" s="25"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" s="27"/>
-      <c r="B82" s="27"/>
-      <c r="C82" s="27"/>
+      <c r="A82" s="26"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="15"/>
       <c r="L82" s="15"/>
-      <c r="M82" s="22"/>
+      <c r="M82" s="25"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A83" s="27" t="s">
+      <c r="A83" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="B83" s="27" t="s">
+      <c r="B83" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="C83" s="27"/>
+      <c r="C83" s="26"/>
       <c r="D83" s="1" t="s">
         <v>287</v>
       </c>
@@ -5626,9 +5626,9 @@
       <c r="M83" s="13"/>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A84" s="27"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
+      <c r="A84" s="26"/>
+      <c r="B84" s="26"/>
+      <c r="C84" s="26"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="I84" s="1"/>
@@ -5637,9 +5637,9 @@
       <c r="M84" s="13"/>
     </row>
     <row r="85" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="27"/>
-      <c r="B85" s="27"/>
-      <c r="C85" s="27"/>
+      <c r="A85" s="26"/>
+      <c r="B85" s="26"/>
+      <c r="C85" s="26"/>
       <c r="D85" s="1" t="s">
         <v>197</v>
       </c>
@@ -5653,13 +5653,13 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="27" t="s">
+      <c r="A86" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="B86" s="27" t="s">
+      <c r="B86" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="C86" s="27" t="s">
+      <c r="C86" s="26" t="s">
         <v>235</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -5672,14 +5672,14 @@
       <c r="L86" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M86" s="23" t="s">
+      <c r="M86" s="24" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="27"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
+      <c r="A87" s="26"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
       <c r="D87" s="1" t="s">
         <v>153</v>
       </c>
@@ -5690,62 +5690,62 @@
       <c r="L87" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="M87" s="22"/>
+      <c r="M87" s="25"/>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="27"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
+      <c r="A88" s="26"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="I88" s="1"/>
       <c r="J88" s="15"/>
       <c r="L88" s="15"/>
-      <c r="M88" s="22"/>
+      <c r="M88" s="25"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="27"/>
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
+      <c r="A89" s="26"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="15"/>
       <c r="L89" s="15"/>
-      <c r="M89" s="22"/>
+      <c r="M89" s="25"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="27"/>
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
+      <c r="A90" s="26"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="21"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="15"/>
       <c r="L90" s="15"/>
-      <c r="M90" s="22"/>
+      <c r="M90" s="25"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" s="27"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
+      <c r="A91" s="26"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="21"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="15"/>
       <c r="L91" s="15"/>
-      <c r="M91" s="22"/>
+      <c r="M91" s="25"/>
     </row>
     <row r="92" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>344</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
@@ -5753,7 +5753,7 @@
       </c>
       <c r="E92" s="1"/>
       <c r="L92" s="15" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.25">
@@ -5815,14 +5815,52 @@
   </sheetData>
   <autoFilter ref="A1:M91" xr:uid="{FE8A9026-FDB0-4A8E-BB8F-FE98E3487D08}"/>
   <mergeCells count="70">
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="C10:C16"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="M77:M78"/>
+    <mergeCell ref="M79:M82"/>
+    <mergeCell ref="M4:M8"/>
+    <mergeCell ref="M10:M16"/>
+    <mergeCell ref="M17:M25"/>
+    <mergeCell ref="M26:M29"/>
+    <mergeCell ref="M30:M37"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A17:A25"/>
+    <mergeCell ref="A10:A16"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="M86:M91"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="M40:M54"/>
+    <mergeCell ref="M55:M64"/>
+    <mergeCell ref="M65:M68"/>
+    <mergeCell ref="M69:M76"/>
+    <mergeCell ref="B17:B25"/>
+    <mergeCell ref="C17:C25"/>
+    <mergeCell ref="F4:F8"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="B30:B37"/>
+    <mergeCell ref="C30:C37"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A54"/>
+    <mergeCell ref="A55:A64"/>
+    <mergeCell ref="A69:A76"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="B86:B91"/>
+    <mergeCell ref="A83:A85"/>
     <mergeCell ref="C86:C91"/>
     <mergeCell ref="C77:C78"/>
     <mergeCell ref="B38:B39"/>
@@ -5839,52 +5877,14 @@
     <mergeCell ref="C69:C76"/>
     <mergeCell ref="B77:B78"/>
     <mergeCell ref="B83:B85"/>
-    <mergeCell ref="A69:A76"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="B86:B91"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="C26:C29"/>
-    <mergeCell ref="B30:B37"/>
-    <mergeCell ref="C30:C37"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A54"/>
-    <mergeCell ref="A55:A64"/>
-    <mergeCell ref="B17:B25"/>
-    <mergeCell ref="C17:C25"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="M86:M91"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M40:M54"/>
-    <mergeCell ref="M55:M64"/>
-    <mergeCell ref="M65:M68"/>
-    <mergeCell ref="M69:M76"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="M77:M78"/>
-    <mergeCell ref="M79:M82"/>
-    <mergeCell ref="M4:M8"/>
-    <mergeCell ref="M10:M16"/>
-    <mergeCell ref="M17:M25"/>
-    <mergeCell ref="M26:M29"/>
-    <mergeCell ref="M30:M37"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="A17:A25"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="C4:C9"/>
-    <mergeCell ref="B10:B16"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="C10:C16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" display="https://www.nuplazidhcp.com/about-pd-psychosis" xr:uid="{00000000-0004-0000-0200-000000000000}"/>

</xml_diff>